<commit_message>
- Designators placed for Assembly file - Serigraphy (authors, date)
</commit_message>
<xml_diff>
--- a/V2/HW/Power/Project Outputs for PowerUnit/PowerUnit.xlsx
+++ b/V2/HW/Power/Project Outputs for PowerUnit/PowerUnit.xlsx
@@ -846,7 +846,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,13 +1209,13 @@
         <v>59</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Added teardrops on header nets - Updated BoM - PCB validated on EC checker
</commit_message>
<xml_diff>
--- a/V2/HW/Power/Project Outputs for PowerUnit/PowerUnit.xlsx
+++ b/V2/HW/Power/Project Outputs for PowerUnit/PowerUnit.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t>Designator</t>
   </si>
@@ -79,7 +79,7 @@
     <t>GRM188R72A103KA01D</t>
   </si>
   <si>
-    <t xml:space="preserve">490-6438-1-ND </t>
+    <t>490-6438-1-ND</t>
   </si>
   <si>
     <t>C25, C29</t>
@@ -208,7 +208,7 @@
     <t>1869279</t>
   </si>
   <si>
-    <t xml:space="preserve">277-5855-ND </t>
+    <t>277-5855-ND</t>
   </si>
   <si>
     <t>P3</t>
@@ -217,9 +217,6 @@
     <t>Header, 10-Pin</t>
   </si>
   <si>
-    <t xml:space="preserve">277-1810-ND </t>
-  </si>
-  <si>
     <t>R1, R2, R3, R4, R9, R10, R11, R12, R17, R18</t>
   </si>
   <si>
@@ -259,7 +256,7 @@
     <t>ERJ-6ENF22R0V</t>
   </si>
   <si>
-    <t xml:space="preserve">P22.0CCT-ND </t>
+    <t>P22.0CCT-ND</t>
   </si>
   <si>
     <t>R25, R28</t>
@@ -268,7 +265,7 @@
     <t>Susumu</t>
   </si>
   <si>
-    <t xml:space="preserve">RR0510P-104-D </t>
+    <t>RR0510P-104-D</t>
   </si>
   <si>
     <t>RR05P100KDCT-ND</t>
@@ -304,13 +301,13 @@
     <t>ESR10EZPJ223</t>
   </si>
   <si>
-    <t xml:space="preserve">RHM22KKCT-ND </t>
+    <t>RHM22KKCT-ND</t>
   </si>
   <si>
     <t>R33, R39</t>
   </si>
   <si>
-    <t xml:space="preserve">RR0510P-103-D </t>
+    <t>RR0510P-103-D</t>
   </si>
   <si>
     <t>RR05P10.0KDCT-ND</t>
@@ -409,7 +406,7 @@
     <t>Texas Intruments</t>
   </si>
   <si>
-    <t xml:space="preserve">LM5106MM/NOPB </t>
+    <t>LM5106MM/NOPB</t>
   </si>
   <si>
     <t>LM5106MM/NOPBCT-ND</t>
@@ -430,7 +427,7 @@
     <t>U9</t>
   </si>
   <si>
-    <t xml:space="preserve">74AHC1G32SE-7 </t>
+    <t>74AHC1G32SE-7</t>
   </si>
   <si>
     <t>74AHC1G32SE-7DICT-ND</t>
@@ -467,12 +464,6 @@
   </si>
   <si>
     <t>MCP9501PT-095E/OTCT-ND</t>
-  </si>
-  <si>
-    <t>Quantity*2</t>
-  </si>
-  <si>
-    <t>Quantity*3</t>
   </si>
 </sst>
 </file>
@@ -843,18 +834,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,14 +862,8 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -899,14 +882,8 @@
       <c r="F2" s="3">
         <v>2</v>
       </c>
-      <c r="G2" s="3">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -925,14 +902,8 @@
       <c r="F3" s="3">
         <v>7</v>
       </c>
-      <c r="G3" s="3">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -951,14 +922,8 @@
       <c r="F4" s="3">
         <v>15</v>
       </c>
-      <c r="G4" s="3">
-        <v>30</v>
-      </c>
-      <c r="H4" s="3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -977,14 +942,8 @@
       <c r="F5" s="3">
         <v>14</v>
       </c>
-      <c r="G5" s="3">
-        <v>28</v>
-      </c>
-      <c r="H5" s="3">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1003,14 +962,8 @@
       <c r="F6" s="3">
         <v>2</v>
       </c>
-      <c r="G6" s="3">
-        <v>4</v>
-      </c>
-      <c r="H6" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1029,14 +982,8 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="3">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -1055,14 +1002,8 @@
       <c r="F8" s="3">
         <v>12</v>
       </c>
-      <c r="G8" s="3">
-        <v>24</v>
-      </c>
-      <c r="H8" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1081,14 +1022,8 @@
       <c r="F9" s="3">
         <v>5</v>
       </c>
-      <c r="G9" s="3">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
@@ -1107,14 +1042,8 @@
       <c r="F10" s="3">
         <v>2</v>
       </c>
-      <c r="G10" s="3">
-        <v>4</v>
-      </c>
-      <c r="H10" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1133,14 +1062,8 @@
       <c r="F11" s="3">
         <v>2</v>
       </c>
-      <c r="G11" s="3">
-        <v>4</v>
-      </c>
-      <c r="H11" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1159,14 +1082,8 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="3">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1185,14 +1102,8 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -1209,16 +1120,10 @@
         <v>59</v>
       </c>
       <c r="F14" s="3">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3">
-        <v>4</v>
-      </c>
-      <c r="H14" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
@@ -1237,14 +1142,8 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="3">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1258,489 +1157,375 @@
         <v>58</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
-      <c r="G16" s="3">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="F17" s="3">
         <v>10</v>
       </c>
-      <c r="G17" s="3">
-        <v>20</v>
-      </c>
-      <c r="H17" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="F18" s="3">
         <v>16</v>
       </c>
-      <c r="G18" s="3">
-        <v>32</v>
-      </c>
-      <c r="H18" s="3">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F19" s="3">
         <v>2</v>
       </c>
-      <c r="G19" s="3">
-        <v>4</v>
-      </c>
-      <c r="H19" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="F20" s="3">
         <v>4</v>
       </c>
-      <c r="G20" s="3">
-        <v>8</v>
-      </c>
-      <c r="H20" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G21" s="3">
-        <v>4</v>
-      </c>
-      <c r="H21" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="F22" s="3">
         <v>2</v>
       </c>
-      <c r="G22" s="3">
-        <v>4</v>
-      </c>
-      <c r="H22" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F23" s="3">
         <v>2</v>
       </c>
-      <c r="G23" s="3">
-        <v>4</v>
-      </c>
-      <c r="H23" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F24" s="3">
         <v>2</v>
       </c>
-      <c r="G24" s="3">
-        <v>4</v>
-      </c>
-      <c r="H24" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="3">
         <v>2</v>
       </c>
-      <c r="G25" s="3">
-        <v>4</v>
-      </c>
-      <c r="H25" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="3">
-        <v>2</v>
-      </c>
-      <c r="H26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="F27" s="3">
         <v>4</v>
       </c>
-      <c r="G27" s="3">
-        <v>8</v>
-      </c>
-      <c r="H27" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="3">
-        <v>2</v>
-      </c>
-      <c r="H28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G29" s="3">
-        <v>2</v>
-      </c>
-      <c r="H29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="F30" s="3">
         <v>3</v>
       </c>
-      <c r="G30" s="3">
-        <v>6</v>
-      </c>
-      <c r="H30" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
-      <c r="G31" s="3">
-        <v>2</v>
-      </c>
-      <c r="H31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
       </c>
-      <c r="G32" s="3">
-        <v>2</v>
-      </c>
-      <c r="H32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="F33" s="3">
         <v>2</v>
       </c>
-      <c r="G33" s="3">
-        <v>4</v>
-      </c>
-      <c r="H33" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
       </c>
-      <c r="G34" s="3">
-        <v>2</v>
-      </c>
-      <c r="H34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>7</v>
@@ -1749,97 +1534,73 @@
         <v>35</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
-      <c r="G35" s="3">
-        <v>2</v>
-      </c>
-      <c r="H35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="F36" s="3">
         <v>2</v>
       </c>
-      <c r="G36" s="3">
-        <v>4</v>
-      </c>
-      <c r="H36" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
-      <c r="G37" s="3">
-        <v>2</v>
-      </c>
-      <c r="H37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
-      </c>
-      <c r="G38" s="3">
-        <v>2</v>
-      </c>
-      <c r="H38" s="3">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Schematic done - PDF generated - BOM OK - GERBER generated - FAB folder created and fulfilled - V2 considered as stable and completed
</commit_message>
<xml_diff>
--- a/V2/HW/Power/Project Outputs for PowerUnit/PowerUnit.xlsx
+++ b/V2/HW/Power/Project Outputs for PowerUnit/PowerUnit.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="152">
   <si>
     <t>Designator</t>
   </si>
@@ -76,10 +76,13 @@
     <t>C9, C10, C11, C12, C15, C16, C17, C18, C19, C20, C37, C38, C39, C40</t>
   </si>
   <si>
-    <t>GRM188R72A103KA01D</t>
-  </si>
-  <si>
-    <t>490-6438-1-ND</t>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>CL10B683KB8NNNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-1814-1-ND </t>
   </si>
   <si>
     <t>C25, C29</t>
@@ -464,6 +467,9 @@
   </si>
   <si>
     <t>MCP9501PT-095E/OTCT-ND</t>
+  </si>
+  <si>
+    <t>Quantity*2</t>
   </si>
 </sst>
 </file>
@@ -834,16 +840,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="18" customWidth="1"/>
+    <col min="1" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,8 +870,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -882,8 +893,11 @@
       <c r="F2" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -902,8 +916,11 @@
       <c r="F3" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -922,8 +939,11 @@
       <c r="F4" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -931,21 +951,24 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -954,653 +977,752 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F17" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F19" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F27" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F33" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F36" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>